<commit_message>
update path for exe
</commit_message>
<xml_diff>
--- a/팀_구성_결과.xlsx
+++ b/팀_구성_결과.xlsx
@@ -23,6 +23,9 @@
     <t>t2</t>
   </si>
   <si>
+    <t>고광민</t>
+  </si>
+  <si>
     <t>김동민</t>
   </si>
   <si>
@@ -50,25 +53,22 @@
     <t>강명석</t>
   </si>
   <si>
+    <t>허기언</t>
+  </si>
+  <si>
+    <t>안준혁</t>
+  </si>
+  <si>
+    <t>이석원</t>
+  </si>
+  <si>
+    <t>소동섭</t>
+  </si>
+  <si>
+    <t>김민성A</t>
+  </si>
+  <si>
     <t>이홍관</t>
-  </si>
-  <si>
-    <t>허기언</t>
-  </si>
-  <si>
-    <t>안준혁</t>
-  </si>
-  <si>
-    <t>이석원</t>
-  </si>
-  <si>
-    <t>고광민</t>
-  </si>
-  <si>
-    <t>소동섭</t>
-  </si>
-  <si>
-    <t>김민성A</t>
   </si>
   <si>
     <t>안지운</t>
@@ -146,18 +146,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFE4E1"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -193,13 +187,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -616,23 +609,23 @@
       <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="2"/>
+      <c r="B15" s="2" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>31</v>
+      <c r="B16" s="2" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>32</v>
-      </c>
+      <c r="B17" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -660,7 +653,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
         <v>31</v>
@@ -671,7 +664,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>30</v>
@@ -682,7 +675,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
         <v>29</v>
@@ -693,7 +686,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>28</v>
@@ -704,7 +697,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
         <v>27</v>
@@ -715,7 +708,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
         <v>26</v>
@@ -726,7 +719,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
         <v>25</v>
@@ -737,32 +730,32 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:3">

</xml_diff>